<commit_message>
Updated MySQL configuration to use environment variables
</commit_message>
<xml_diff>
--- a/static/uploads/sample_format_excel.xlsx
+++ b/static/uploads/sample_format_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohitkoli/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA40A5E2-6398-8245-B40F-242100D7DBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27EC651-12FE-4D43-B908-1C8AB43E3A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Roll No</t>
   </si>
@@ -58,13 +58,7 @@
     <t>koli</t>
   </si>
   <si>
-    <t>mohitkoli@gmail.com</t>
-  </si>
-  <si>
-    <t>22101B0022</t>
-  </si>
-  <si>
-    <t>mohit</t>
+    <t>mohitkoli1234@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -446,7 +440,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -482,8 +476,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>13</v>
+      <c r="A2">
+        <v>1234</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -494,8 +488,8 @@
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
+      <c r="E2">
+        <v>123</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>

</xml_diff>